<commit_message>
completed a simple supplie system
</commit_message>
<xml_diff>
--- a/Assets/_Excel/dialogue.xlsx
+++ b/Assets/_Excel/dialogue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unity\BattleFlagGameStudy\Assets\_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B443FD9-3800-4EB8-B659-9D31728BFFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039BABD0-D764-40E3-958B-79033E960D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7140" yWindow="2160" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="495" yWindow="2565" windowWidth="27675" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -144,6 +144,14 @@
   </si>
   <si>
     <t>icon/up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩家交互</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -469,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -660,6 +668,35 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>10005</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7">
+        <v>10001</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>